<commit_message>
Add new features and tutorials without tracking videos
</commit_message>
<xml_diff>
--- a/templates/adaa.xlsx
+++ b/templates/adaa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\modax\Desktop\AJYAL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\new\SchoolRanker\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BB011F8-F1BB-4601-8365-1B4E8E21E6EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8279F10-D47F-4F09-B2C0-FB2E5B729ABD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{59F9A634-5C70-4D1F-83F5-5E22FB022DD4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{59F9A634-5C70-4D1F-83F5-5E22FB022DD4}"/>
   </bookViews>
   <sheets>
     <sheet name="(1)" sheetId="1" r:id="rId1"/>
@@ -91,7 +91,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -110,26 +110,20 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
+      <sz val="8"/>
       <name val="Arial"/>
-      <family val="2"/>
+      <charset val="178"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Inherit"/>
-      <charset val="178"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
       <charset val="178"/>
     </font>
   </fonts>
@@ -141,7 +135,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -164,61 +158,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_ورقة1" xfId="1" xr:uid="{1B6EEF7B-442E-4614-8D8F-F1551E0C4715}"/>
+    <cellStyle name="عادي" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -522,85 +536,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{023347E5-B369-4FF1-9B6E-0A727279EF53}">
   <dimension ref="A1:U66"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScale="130" zoomScaleNormal="75" zoomScaleSheetLayoutView="130" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView rightToLeft="1" tabSelected="1" view="pageBreakPreview" zoomScaleNormal="75" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="18"/>
   <cols>
     <col min="1" max="1" width="5" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="6.6640625" style="2" customWidth="1"/>
-    <col min="5" max="8" width="4.44140625" style="2" customWidth="1"/>
-    <col min="9" max="20" width="4.5546875" style="2" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" style="2" customWidth="1"/>
-    <col min="22" max="16384" width="9.109375" style="1"/>
+    <col min="2" max="2" width="26.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="6.7109375" style="2" customWidth="1"/>
+    <col min="5" max="8" width="4.42578125" style="2" customWidth="1"/>
+    <col min="9" max="20" width="4.5703125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18.75" customHeight="1">
-      <c r="A1" s="6"/>
-      <c r="B1" s="6"/>
-      <c r="C1" s="7" t="s">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="5"/>
-      <c r="U1" s="7" t="s">
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="18" customHeight="1">
-      <c r="A2" s="8"/>
-      <c r="B2" s="9"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="5" t="s">
+      <c r="A2" s="9"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="7"/>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+      <c r="M2" s="7"/>
+      <c r="N2" s="7"/>
+      <c r="O2" s="7"/>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="8"/>
     </row>
     <row r="3" spans="1:21" ht="36.75" customHeight="1">
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
@@ -617,585 +631,582 @@
       <c r="R3" s="11"/>
       <c r="S3" s="11"/>
       <c r="T3" s="11"/>
-      <c r="U3" s="7"/>
+      <c r="U3" s="8"/>
     </row>
     <row r="4" spans="1:21" ht="41.25" customHeight="1">
-      <c r="B4" s="12" t="s">
+      <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="13" t="s">
+      <c r="B4" s="6"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="G4" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="13" t="s">
+      <c r="H4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="N4" s="14" t="s">
+      <c r="N4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="O4" s="14" t="s">
+      <c r="O4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="14" t="s">
+      <c r="P4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="14" t="s">
+      <c r="Q4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="S4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="14" t="s">
+      <c r="T4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="7"/>
+      <c r="U4" s="8"/>
     </row>
     <row r="5" spans="1:21">
       <c r="A5" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="13"/>
-      <c r="H5" s="13"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="14"/>
-      <c r="N5" s="14"/>
-      <c r="O5" s="14"/>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="15"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+      <c r="L5" s="8"/>
+      <c r="M5" s="8"/>
+      <c r="N5" s="8"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="8"/>
+      <c r="Q5" s="8"/>
+      <c r="R5" s="8"/>
+      <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
+      <c r="U5" s="3"/>
     </row>
     <row r="6" spans="1:21" ht="26.25" customHeight="1">
       <c r="A6" s="2">
         <v>1</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
     </row>
     <row r="7" spans="1:21" ht="26.25" customHeight="1">
       <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
+      <c r="B7" s="13"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:21" ht="26.25" customHeight="1">
       <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
     </row>
     <row r="9" spans="1:21" ht="26.25" customHeight="1">
       <c r="A9" s="2">
         <v>4</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="16"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:21" ht="26.25" customHeight="1">
       <c r="A10" s="2">
         <v>5</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="16"/>
-      <c r="D10" s="16"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
     <row r="11" spans="1:21" ht="26.25" customHeight="1">
       <c r="A11" s="2">
         <v>6</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="16"/>
-      <c r="D11" s="16"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
     </row>
     <row r="12" spans="1:21" ht="26.25" customHeight="1">
       <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="16"/>
-      <c r="D12" s="16"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:21" ht="26.25" customHeight="1">
       <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="B13" s="3"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="1:21" ht="26.25" customHeight="1">
       <c r="A14" s="2">
         <v>9</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:21" ht="26.25" customHeight="1">
       <c r="A15" s="2">
         <v>10</v>
       </c>
-      <c r="B15" s="3"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:21" ht="26.25" customHeight="1">
       <c r="A16" s="2">
         <v>11</v>
       </c>
-      <c r="B16" s="3"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
     </row>
     <row r="17" spans="1:4" ht="26.25" customHeight="1">
       <c r="A17" s="2">
         <v>12</v>
       </c>
-      <c r="B17" s="3"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
     </row>
     <row r="18" spans="1:4" ht="26.25" customHeight="1">
       <c r="A18" s="2">
         <v>13</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="16"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="26.25" customHeight="1">
       <c r="A19" s="2">
         <v>14</v>
       </c>
-      <c r="B19" s="3"/>
-      <c r="C19" s="16"/>
-      <c r="D19" s="16"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
     </row>
     <row r="20" spans="1:4" ht="26.25" customHeight="1">
       <c r="A20" s="2">
         <v>15</v>
       </c>
-      <c r="B20" s="3"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
     </row>
     <row r="21" spans="1:4" ht="26.25" customHeight="1">
       <c r="A21" s="2">
         <v>16</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
+      <c r="B21" s="13"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
     </row>
     <row r="22" spans="1:4" ht="26.25" customHeight="1">
       <c r="A22" s="2">
         <v>17</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="16"/>
-      <c r="D22" s="16"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" ht="26.25" customHeight="1">
       <c r="A23" s="2">
         <v>18</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="16"/>
-      <c r="D23" s="16"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" ht="26.25" customHeight="1">
       <c r="A24" s="2">
         <v>19</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="16"/>
-      <c r="D24" s="16"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
     </row>
     <row r="25" spans="1:4" ht="26.25" customHeight="1">
       <c r="A25" s="2">
         <v>20</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="16"/>
-      <c r="D25" s="16"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" ht="26.25" customHeight="1">
       <c r="A26" s="2">
         <v>21</v>
       </c>
-      <c r="B26" s="3"/>
-      <c r="C26" s="16"/>
-      <c r="D26" s="16"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" ht="26.25" customHeight="1">
       <c r="A27" s="2">
         <v>22</v>
       </c>
-      <c r="B27" s="3"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="16"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" ht="26.25" customHeight="1">
       <c r="A28" s="2">
         <v>23</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="16"/>
-      <c r="D28" s="16"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
     </row>
     <row r="29" spans="1:4" ht="26.25" customHeight="1">
       <c r="A29" s="2">
         <v>24</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="16"/>
-      <c r="D29" s="16"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" ht="26.25" customHeight="1">
       <c r="A30" s="2">
         <v>25</v>
       </c>
-      <c r="B30" s="3"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
     </row>
     <row r="31" spans="1:4" ht="26.25" customHeight="1">
       <c r="A31" s="2">
         <v>26</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="16"/>
-      <c r="D31" s="16"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
     </row>
     <row r="32" spans="1:4" ht="26.25" customHeight="1">
       <c r="A32" s="2">
         <v>27</v>
       </c>
-      <c r="B32" s="3"/>
-      <c r="C32" s="16"/>
-      <c r="D32" s="16"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
     </row>
     <row r="33" spans="1:4" ht="26.25" customHeight="1">
       <c r="A33" s="2">
         <v>28</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
     </row>
     <row r="34" spans="1:4" ht="26.25" customHeight="1">
       <c r="A34" s="2">
         <v>29</v>
       </c>
-      <c r="B34" s="3"/>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
+      <c r="B34" s="13"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
     </row>
     <row r="35" spans="1:4" ht="26.25" customHeight="1">
       <c r="A35" s="2">
         <v>30</v>
       </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="16"/>
-      <c r="D35" s="16"/>
+      <c r="B35" s="13"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
     </row>
     <row r="36" spans="1:4" ht="26.25" customHeight="1">
       <c r="A36" s="2">
         <v>31</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="16"/>
-      <c r="D36" s="16"/>
+      <c r="B36" s="13"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
     </row>
     <row r="37" spans="1:4" ht="26.25" customHeight="1">
       <c r="A37" s="2">
         <v>32</v>
       </c>
-      <c r="B37" s="3"/>
-      <c r="C37" s="16"/>
-      <c r="D37" s="16"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
     </row>
     <row r="38" spans="1:4" ht="26.25" customHeight="1">
       <c r="A38" s="2">
         <v>33</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="16"/>
-      <c r="D38" s="16"/>
+      <c r="B38" s="13"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
     </row>
     <row r="39" spans="1:4" ht="26.25" customHeight="1">
       <c r="A39" s="2">
         <v>34</v>
       </c>
-      <c r="B39" s="3"/>
-      <c r="C39" s="16"/>
-      <c r="D39" s="16"/>
+      <c r="B39" s="13"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
     </row>
     <row r="40" spans="1:4" ht="26.25" customHeight="1">
       <c r="A40" s="2">
         <v>35</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="16"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
     </row>
     <row r="41" spans="1:4" ht="26.25" customHeight="1">
       <c r="A41" s="2">
         <v>36</v>
       </c>
-      <c r="B41" s="3"/>
-      <c r="C41" s="16"/>
-      <c r="D41" s="16"/>
+      <c r="B41" s="13"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
     </row>
     <row r="42" spans="1:4" ht="26.25" customHeight="1">
       <c r="A42" s="2">
         <v>37</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="16"/>
-      <c r="D42" s="16"/>
+      <c r="B42" s="13"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
     </row>
     <row r="43" spans="1:4" ht="26.25" customHeight="1">
       <c r="A43" s="2">
         <v>38</v>
       </c>
-      <c r="B43" s="3"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="16"/>
+      <c r="B43" s="13"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
     </row>
     <row r="44" spans="1:4" ht="26.25" customHeight="1">
       <c r="A44" s="2">
         <v>39</v>
       </c>
-      <c r="B44" s="3"/>
-      <c r="C44" s="16"/>
-      <c r="D44" s="16"/>
+      <c r="B44" s="13"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
     </row>
     <row r="45" spans="1:4" ht="26.25" customHeight="1">
       <c r="A45" s="2">
         <v>40</v>
       </c>
-      <c r="B45" s="3"/>
-      <c r="C45" s="16"/>
-      <c r="D45" s="16"/>
+      <c r="B45" s="13"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
     </row>
     <row r="46" spans="1:4" ht="26.25" customHeight="1">
       <c r="A46" s="2">
         <v>41</v>
       </c>
-      <c r="B46" s="3"/>
-      <c r="C46" s="16"/>
-      <c r="D46" s="16"/>
+      <c r="B46" s="13"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
     </row>
     <row r="47" spans="1:4" ht="26.25" customHeight="1">
       <c r="A47" s="2">
         <v>42</v>
       </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="16"/>
-      <c r="D47" s="16"/>
+      <c r="B47" s="13"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
     </row>
     <row r="48" spans="1:4" ht="26.25" customHeight="1">
       <c r="A48" s="2">
         <v>43</v>
       </c>
-      <c r="B48" s="3"/>
-      <c r="C48" s="16"/>
-      <c r="D48" s="16"/>
+      <c r="B48" s="13"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
     </row>
     <row r="49" spans="1:4" ht="26.25" customHeight="1">
       <c r="A49" s="2">
         <v>44</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="16"/>
-      <c r="D49" s="16"/>
+      <c r="B49" s="13"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
     </row>
     <row r="50" spans="1:4" ht="26.25" customHeight="1">
       <c r="A50" s="2">
         <v>45</v>
       </c>
-      <c r="B50" s="3"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="16"/>
+      <c r="B50" s="13"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="4"/>
     </row>
     <row r="51" spans="1:4" ht="26.25" customHeight="1">
       <c r="A51" s="2">
         <v>46</v>
       </c>
-      <c r="B51" s="3"/>
-      <c r="C51" s="16"/>
-      <c r="D51" s="16"/>
+      <c r="B51" s="13"/>
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
     </row>
     <row r="52" spans="1:4" ht="26.25" customHeight="1">
       <c r="A52" s="2">
         <v>47</v>
       </c>
-      <c r="B52" s="3"/>
-      <c r="C52" s="16"/>
-      <c r="D52" s="16"/>
+      <c r="B52" s="13"/>
+      <c r="C52" s="4"/>
+      <c r="D52" s="4"/>
     </row>
     <row r="53" spans="1:4" ht="26.25" customHeight="1">
       <c r="A53" s="2">
         <v>48</v>
       </c>
-      <c r="B53" s="3"/>
-      <c r="C53" s="16"/>
-      <c r="D53" s="16"/>
+      <c r="B53" s="13"/>
+      <c r="C53" s="4"/>
+      <c r="D53" s="4"/>
     </row>
     <row r="54" spans="1:4" ht="26.25" customHeight="1">
       <c r="A54" s="2">
         <v>49</v>
       </c>
-      <c r="B54" s="3"/>
-      <c r="C54" s="16"/>
-      <c r="D54" s="16"/>
+      <c r="B54" s="13"/>
+      <c r="C54" s="4"/>
+      <c r="D54" s="4"/>
     </row>
     <row r="55" spans="1:4" ht="26.25" customHeight="1">
       <c r="A55" s="2">
         <v>50</v>
       </c>
-      <c r="B55" s="3"/>
-      <c r="C55" s="16"/>
-      <c r="D55" s="16"/>
+      <c r="B55" s="13"/>
+      <c r="C55" s="4"/>
+      <c r="D55" s="4"/>
     </row>
     <row r="56" spans="1:4" ht="26.25" customHeight="1">
       <c r="A56" s="2">
         <v>51</v>
       </c>
-      <c r="B56" s="3"/>
-      <c r="C56" s="16"/>
-      <c r="D56" s="16"/>
+      <c r="B56" s="13"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
     </row>
     <row r="57" spans="1:4" ht="26.25" customHeight="1">
       <c r="A57" s="2">
         <v>52</v>
       </c>
-      <c r="B57" s="3"/>
-      <c r="C57" s="16"/>
-      <c r="D57" s="16"/>
+      <c r="B57" s="13"/>
+      <c r="C57" s="4"/>
+      <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" ht="26.25" customHeight="1">
       <c r="A58" s="2">
         <v>53</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="16"/>
-      <c r="D58" s="16"/>
+      <c r="B58" s="13"/>
+      <c r="C58" s="4"/>
+      <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" ht="26.25" customHeight="1">
       <c r="A59" s="2">
         <v>54</v>
       </c>
-      <c r="B59" s="3"/>
-      <c r="C59" s="16"/>
-      <c r="D59" s="16"/>
+      <c r="B59" s="13"/>
+      <c r="C59" s="4"/>
+      <c r="D59" s="4"/>
     </row>
     <row r="60" spans="1:4" ht="26.25" customHeight="1">
       <c r="A60" s="2">
         <v>55</v>
       </c>
-      <c r="B60" s="3"/>
-      <c r="C60" s="16"/>
-      <c r="D60" s="16"/>
+      <c r="B60" s="13"/>
+      <c r="C60" s="4"/>
+      <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" ht="26.25" customHeight="1">
       <c r="A61" s="2">
         <v>56</v>
       </c>
-      <c r="B61" s="3"/>
-      <c r="C61" s="16"/>
-      <c r="D61" s="16"/>
+      <c r="B61" s="13"/>
+      <c r="C61" s="4"/>
+      <c r="D61" s="4"/>
     </row>
     <row r="62" spans="1:4" ht="26.25" customHeight="1">
       <c r="A62" s="2">
         <v>57</v>
       </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="16"/>
-      <c r="D62" s="16"/>
+      <c r="B62" s="13"/>
+      <c r="C62" s="4"/>
+      <c r="D62" s="4"/>
     </row>
     <row r="63" spans="1:4" ht="26.25" customHeight="1">
       <c r="A63" s="2">
         <v>58</v>
       </c>
-      <c r="B63" s="3"/>
-      <c r="C63" s="16"/>
-      <c r="D63" s="16"/>
+      <c r="B63" s="13"/>
+      <c r="C63" s="4"/>
+      <c r="D63" s="4"/>
     </row>
     <row r="64" spans="1:4" ht="26.25" customHeight="1">
       <c r="A64" s="2">
         <v>59</v>
       </c>
-      <c r="B64" s="3"/>
-      <c r="C64" s="16"/>
-      <c r="D64" s="16"/>
+      <c r="B64" s="13"/>
+      <c r="C64" s="4"/>
+      <c r="D64" s="4"/>
     </row>
     <row r="65" spans="1:4" ht="26.25" customHeight="1">
       <c r="A65" s="2">
         <v>60</v>
       </c>
-      <c r="B65" s="3"/>
-      <c r="C65" s="16"/>
-      <c r="D65" s="16"/>
+      <c r="B65" s="13"/>
+      <c r="C65" s="4"/>
+      <c r="D65" s="4"/>
     </row>
     <row r="66" spans="1:4" ht="26.25" customHeight="1">
       <c r="A66" s="2">
         <v>61</v>
       </c>
-      <c r="B66" s="3"/>
-      <c r="C66" s="16"/>
-      <c r="D66" s="16"/>
+      <c r="B66" s="13"/>
+      <c r="C66" s="4"/>
+      <c r="D66" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="29">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:C5"/>
-    <mergeCell ref="D1:D5"/>
-    <mergeCell ref="E1:T1"/>
+  <mergeCells count="30">
     <mergeCell ref="U1:U4"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="E2:H2"/>
@@ -1212,6 +1223,11 @@
     <mergeCell ref="I4:I5"/>
     <mergeCell ref="J4:J5"/>
     <mergeCell ref="K4:K5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:C5"/>
+    <mergeCell ref="D1:D5"/>
+    <mergeCell ref="E1:T1"/>
     <mergeCell ref="R4:R5"/>
     <mergeCell ref="S4:S5"/>
     <mergeCell ref="T4:T5"/>
@@ -1222,7 +1238,7 @@
     <mergeCell ref="P4:P5"/>
     <mergeCell ref="Q4:Q5"/>
   </mergeCells>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.196850393700787" right="0.39370078740157499" top="0.15748031496063" bottom="0.15748031496063" header="0.15748031496063" footer="0.196850393700787"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>